<commit_message>
Agregando el sprint planing 2 y actualizando el cronograma
</commit_message>
<xml_diff>
--- a/Documentos/SF/Cronograma/ST-CP.xlsx
+++ b/Documentos/SF/Cronograma/ST-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jota\Documents\DESARROLLO JOLLJA\FiveSolutions\Documentos\SF\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1699A1C-9BD2-4FA3-B386-7619FBC762F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2884BAB-995C-46D7-B701-6238E45CE018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="150">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -261,9 +261,6 @@
     <t>ST-SP.DOCX</t>
   </si>
   <si>
-    <t>HU-Registrar, actualizar y/o eliminar producto</t>
-  </si>
-  <si>
     <t>Tello/DBA, Benavente/Backend/Centti</t>
   </si>
   <si>
@@ -351,27 +348,12 @@
     <t>HU-Módulo autenticación de usuario</t>
   </si>
   <si>
-    <t>HU-Registrar, editar organización</t>
-  </si>
-  <si>
     <t>HU-Modulo de busqueda</t>
   </si>
   <si>
-    <t>Registrar, editar organización</t>
-  </si>
-  <si>
-    <t>Registrar, actualizar y/o eliminar producto</t>
-  </si>
-  <si>
     <t>Modulo de busqueda</t>
   </si>
   <si>
-    <t>ST-REO.DOCX</t>
-  </si>
-  <si>
-    <t>ST-RAEP.DOCX</t>
-  </si>
-  <si>
     <t>ST-MB.DOCX</t>
   </si>
   <si>
@@ -448,6 +430,51 @@
   </si>
   <si>
     <t>ST-HURO</t>
+  </si>
+  <si>
+    <t>Validar productos y/o servicios</t>
+  </si>
+  <si>
+    <t>ST-VPS.DOCX</t>
+  </si>
+  <si>
+    <t>ST-RAEPS.DOCX</t>
+  </si>
+  <si>
+    <t>HU-Formulario contacto</t>
+  </si>
+  <si>
+    <t>Formulario de Contacto</t>
+  </si>
+  <si>
+    <t>HU-Recuperar Contraseña</t>
+  </si>
+  <si>
+    <t>Recuperar Contraseña</t>
+  </si>
+  <si>
+    <t>ST-RC.DOCX</t>
+  </si>
+  <si>
+    <t>ST-FC.DOCX</t>
+  </si>
+  <si>
+    <t>Registrar, actualizar y/o eliminar producto y/o servicio</t>
+  </si>
+  <si>
+    <t>Zavaleta/DO</t>
+  </si>
+  <si>
+    <t>Benaventa/FBA</t>
+  </si>
+  <si>
+    <t>Israel/TS</t>
+  </si>
+  <si>
+    <t>HU-Registrar, actualizar y/o eliminar producto y/o servicio (Administrador Organizacion)</t>
+  </si>
+  <si>
+    <t>HU-Validar productos y/o servicios (Administrador General)</t>
   </si>
 </sst>
 </file>
@@ -636,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -704,6 +731,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,6 +740,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P1007"/>
+  <dimension ref="B1:P1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C23"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -950,15 +979,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="2:16">
       <c r="B2" s="1" t="s">
@@ -1030,10 +1059,10 @@
       <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="48"/>
+      <c r="K8" s="49"/>
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
@@ -1108,7 +1137,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>25</v>
@@ -1198,16 +1227,16 @@
     </row>
     <row r="14" spans="2:16" s="42" customFormat="1">
       <c r="B14" s="19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1299,7 +1328,7 @@
         <v>53</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F17" s="21">
         <v>44359</v>
@@ -1324,16 +1353,16 @@
     </row>
     <row r="18" spans="2:16">
       <c r="B18" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F18" s="21">
         <v>44363</v>
@@ -1358,13 +1387,13 @@
     </row>
     <row r="19" spans="2:16" s="43" customFormat="1">
       <c r="B19" s="19" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>25</v>
@@ -1388,16 +1417,16 @@
     </row>
     <row r="20" spans="2:16" s="43" customFormat="1">
       <c r="B20" s="19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F20" s="21">
         <v>44363</v>
@@ -1418,13 +1447,13 @@
     </row>
     <row r="21" spans="2:16" s="43" customFormat="1">
       <c r="B21" s="19" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>25</v>
@@ -1448,15 +1477,17 @@
     </row>
     <row r="22" spans="2:16" s="35" customFormat="1">
       <c r="B22" s="19" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="33"/>
+        <v>133</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>145</v>
+      </c>
       <c r="F22" s="21">
         <v>44363</v>
       </c>
@@ -1474,15 +1505,17 @@
     </row>
     <row r="23" spans="2:16" s="35" customFormat="1">
       <c r="B23" s="19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="33"/>
+        <v>134</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>146</v>
+      </c>
       <c r="F23" s="21">
         <v>44363</v>
       </c>
@@ -1509,7 +1542,7 @@
         <v>60</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F24" s="21">
         <v>44367</v>
@@ -1702,10 +1735,10 @@
         <v>25</v>
       </c>
       <c r="F33" s="4">
-        <v>44379</v>
+        <v>44385</v>
       </c>
       <c r="G33" s="4">
-        <v>44380</v>
+        <v>44386</v>
       </c>
       <c r="H33" s="27"/>
     </row>
@@ -1720,124 +1753,124 @@
         <v>77</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F34" s="4">
-        <v>44380</v>
+        <v>44387</v>
       </c>
       <c r="G34" s="4">
-        <v>44383</v>
+        <v>44389</v>
       </c>
       <c r="H34" s="27"/>
     </row>
     <row r="35" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="B35" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>110</v>
+        <v>148</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>144</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" s="33" t="s">
-        <v>56</v>
+        <v>137</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="F35" s="4">
-        <v>44380</v>
+        <v>44391</v>
       </c>
       <c r="G35" s="4">
-        <v>44383</v>
+        <v>44393</v>
       </c>
       <c r="H35" s="27"/>
     </row>
     <row r="36" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="B36" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>111</v>
+        <v>149</v>
+      </c>
+      <c r="C36" s="50" t="s">
+        <v>135</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="33" t="s">
-        <v>56</v>
+        <v>136</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="F36" s="4">
-        <v>44380</v>
+        <v>44391</v>
       </c>
       <c r="G36" s="4">
-        <v>44383</v>
+        <v>44393</v>
       </c>
       <c r="H36" s="27"/>
     </row>
     <row r="37" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="B37" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="33" t="s">
-        <v>56</v>
+      <c r="E37" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="F37" s="4">
-        <v>44380</v>
+        <v>44391</v>
       </c>
       <c r="G37" s="4">
-        <v>44383</v>
+        <v>44393</v>
       </c>
       <c r="H37" s="27"/>
     </row>
-    <row r="38" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B38" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>60</v>
+    <row r="38" spans="2:8" s="45" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B38" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>141</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="21">
-        <v>44397</v>
-      </c>
-      <c r="G38" s="21">
-        <v>44398</v>
+        <v>142</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F38" s="4">
+        <v>44391</v>
+      </c>
+      <c r="G38" s="4">
+        <v>44393</v>
       </c>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B39" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>60</v>
+    <row r="39" spans="2:8" s="45" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B39" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>139</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="21">
-        <v>44398</v>
-      </c>
-      <c r="G39" s="21">
-        <v>44400</v>
+        <v>143</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="4">
+        <v>44391</v>
+      </c>
+      <c r="G39" s="4">
+        <v>44393</v>
       </c>
       <c r="H39" s="27"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" customHeight="1">
       <c r="B40" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>60</v>
@@ -1845,20 +1878,20 @@
       <c r="D40" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="22" t="s">
-        <v>64</v>
+      <c r="E40" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="F40" s="21">
-        <v>44400</v>
+        <v>44397</v>
       </c>
       <c r="G40" s="21">
-        <v>44403</v>
+        <v>44398</v>
       </c>
       <c r="H40" s="27"/>
     </row>
     <row r="41" spans="2:8" ht="15.75" customHeight="1">
       <c r="B41" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>60</v>
@@ -1866,20 +1899,20 @@
       <c r="D41" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="22" t="s">
-        <v>64</v>
+      <c r="E41" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="F41" s="21">
-        <v>44403</v>
+        <v>44398</v>
       </c>
       <c r="G41" s="21">
-        <v>44404</v>
+        <v>44400</v>
       </c>
       <c r="H41" s="27"/>
     </row>
     <row r="42" spans="2:8" ht="15.75" customHeight="1">
       <c r="B42" s="19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>60</v>
@@ -1887,20 +1920,20 @@
       <c r="D42" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>67</v>
+      <c r="E42" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="F42" s="21">
-        <v>44405</v>
+        <v>44400</v>
       </c>
       <c r="G42" s="21">
-        <v>44405</v>
+        <v>44403</v>
       </c>
       <c r="H42" s="27"/>
     </row>
     <row r="43" spans="2:8" ht="15.75" customHeight="1">
       <c r="B43" s="19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>60</v>
@@ -1908,20 +1941,20 @@
       <c r="D43" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="16" t="s">
-        <v>25</v>
+      <c r="E43" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="F43" s="21">
-        <v>44406</v>
+        <v>44403</v>
       </c>
       <c r="G43" s="21">
-        <v>44406</v>
+        <v>44404</v>
       </c>
       <c r="H43" s="27"/>
     </row>
     <row r="44" spans="2:8" ht="15.75" customHeight="1">
       <c r="B44" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>60</v>
@@ -1929,8 +1962,8 @@
       <c r="D44" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="16" t="s">
-        <v>25</v>
+      <c r="E44" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="F44" s="21">
         <v>44405</v>
@@ -1941,141 +1974,141 @@
       <c r="H44" s="27"/>
     </row>
     <row r="45" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="21">
+        <v>44406</v>
+      </c>
+      <c r="G45" s="21">
+        <v>44406</v>
+      </c>
+      <c r="H45" s="27"/>
+    </row>
+    <row r="46" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B46" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="21">
+        <v>44405</v>
+      </c>
+      <c r="G46" s="21">
+        <v>44405</v>
+      </c>
+      <c r="H46" s="27"/>
+    </row>
+    <row r="47" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B47" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="12"/>
+    </row>
+    <row r="48" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B48" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B46" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="13"/>
-    </row>
-    <row r="47" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B47" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="4">
-        <v>44410</v>
-      </c>
-      <c r="G47" s="4">
-        <v>44411</v>
-      </c>
-      <c r="H47" s="27"/>
-    </row>
-    <row r="48" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B48" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F48" s="4">
-        <v>44411</v>
-      </c>
-      <c r="G48" s="4">
-        <v>44414</v>
-      </c>
-      <c r="H48" s="27"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="13"/>
     </row>
     <row r="49" spans="2:8" ht="15.75" customHeight="1">
       <c r="B49" s="16" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="F49" s="21">
-        <v>44417</v>
-      </c>
-      <c r="G49" s="21">
-        <v>44419</v>
+        <v>83</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="4">
+        <v>44410</v>
+      </c>
+      <c r="G49" s="4">
+        <v>44411</v>
       </c>
       <c r="H49" s="27"/>
     </row>
     <row r="50" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B50" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F50" s="21">
-        <v>44424</v>
-      </c>
-      <c r="G50" s="21">
-        <v>44426</v>
+      <c r="B50" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" s="4">
+        <v>44411</v>
+      </c>
+      <c r="G50" s="4">
+        <v>44414</v>
       </c>
       <c r="H50" s="27"/>
     </row>
     <row r="51" spans="2:8" ht="15.75" customHeight="1">
       <c r="B51" s="16" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D51" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E51" s="16" t="s">
-        <v>56</v>
-      </c>
       <c r="F51" s="21">
-        <v>44424</v>
+        <v>44417</v>
       </c>
       <c r="G51" s="21">
-        <v>44426</v>
+        <v>44419</v>
       </c>
       <c r="H51" s="27"/>
     </row>
     <row r="52" spans="2:8" ht="15.75" customHeight="1">
       <c r="B52" s="16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>56</v>
@@ -2090,70 +2123,70 @@
     </row>
     <row r="53" spans="2:8" ht="15.75" customHeight="1">
       <c r="B53" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" s="21">
+        <v>44424</v>
+      </c>
+      <c r="G53" s="21">
+        <v>44426</v>
+      </c>
+      <c r="H53" s="27"/>
+    </row>
+    <row r="54" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B54" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="21">
+        <v>44424</v>
+      </c>
+      <c r="G54" s="21">
+        <v>44426</v>
+      </c>
+      <c r="H54" s="27"/>
+    </row>
+    <row r="55" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B55" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="D55" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="E55" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E53" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F53" s="21">
+      <c r="F55" s="21">
         <v>44426</v>
       </c>
-      <c r="G53" s="21">
+      <c r="G55" s="21">
         <v>44428</v>
-      </c>
-      <c r="H53" s="27"/>
-    </row>
-    <row r="54" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B54" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F54" s="21">
-        <v>44428</v>
-      </c>
-      <c r="G54" s="21">
-        <v>44429</v>
-      </c>
-      <c r="H54" s="27"/>
-    </row>
-    <row r="55" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B55" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F55" s="21">
-        <v>44429</v>
-      </c>
-      <c r="G55" s="21">
-        <v>44431</v>
       </c>
       <c r="H55" s="27"/>
     </row>
     <row r="56" spans="2:8" ht="15.75" customHeight="1">
       <c r="B56" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>60</v>
@@ -2162,19 +2195,19 @@
         <v>60</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="F56" s="21">
-        <v>44431</v>
+        <v>44428</v>
       </c>
       <c r="G56" s="21">
-        <v>44434</v>
+        <v>44429</v>
       </c>
       <c r="H56" s="27"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" customHeight="1">
       <c r="B57" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>60</v>
@@ -2182,20 +2215,20 @@
       <c r="D57" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="22" t="s">
-        <v>64</v>
+      <c r="E57" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="F57" s="21">
-        <v>44434</v>
+        <v>44429</v>
       </c>
       <c r="G57" s="21">
-        <v>44435</v>
+        <v>44431</v>
       </c>
       <c r="H57" s="27"/>
     </row>
     <row r="58" spans="2:8" ht="15.75" customHeight="1">
       <c r="B58" s="19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>60</v>
@@ -2203,20 +2236,20 @@
       <c r="D58" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>67</v>
+      <c r="E58" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="F58" s="21">
-        <v>44436</v>
+        <v>44431</v>
       </c>
       <c r="G58" s="21">
-        <v>44436</v>
+        <v>44434</v>
       </c>
       <c r="H58" s="27"/>
     </row>
     <row r="59" spans="2:8" ht="15.75" customHeight="1">
       <c r="B59" s="19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>60</v>
@@ -2224,20 +2257,20 @@
       <c r="D59" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="16" t="s">
-        <v>25</v>
+      <c r="E59" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="F59" s="21">
-        <v>44437</v>
+        <v>44434</v>
       </c>
       <c r="G59" s="21">
-        <v>44437</v>
+        <v>44435</v>
       </c>
       <c r="H59" s="27"/>
     </row>
     <row r="60" spans="2:8" ht="15.75" customHeight="1">
       <c r="B60" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>60</v>
@@ -2245,8 +2278,8 @@
       <c r="D60" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="16" t="s">
-        <v>25</v>
+      <c r="E60" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="F60" s="21">
         <v>44436</v>
@@ -2257,27 +2290,67 @@
       <c r="H60" s="27"/>
     </row>
     <row r="61" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B61" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="12"/>
+      <c r="B61" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61" s="21">
+        <v>44437</v>
+      </c>
+      <c r="G61" s="21">
+        <v>44437</v>
+      </c>
+      <c r="H61" s="27"/>
     </row>
     <row r="62" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B62" s="12"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="15"/>
-    </row>
-    <row r="63" spans="2:8" ht="15.75" customHeight="1"/>
-    <row r="64" spans="2:8" ht="15.75" customHeight="1"/>
+      <c r="B62" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" s="21">
+        <v>44436</v>
+      </c>
+      <c r="G62" s="21">
+        <v>44436</v>
+      </c>
+      <c r="H62" s="27"/>
+    </row>
+    <row r="63" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B63" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="12"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="12"/>
+    </row>
+    <row r="64" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B64" s="12"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="15"/>
+    </row>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -3221,6 +3294,8 @@
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:H1"/>

</xml_diff>

<commit_message>
Generando los archivos de la Linea Base
</commit_message>
<xml_diff>
--- a/Documentos/SF/Cronograma/ST-CP.xlsx
+++ b/Documentos/SF/Cronograma/ST-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jota\Documents\DESARROLLO JOLLJA\FiveSolutions\Documentos\SF\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2884BAB-995C-46D7-B701-6238E45CE018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17CBDC3-A504-4F7F-AE49-53F8D11F642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,6 +732,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -740,7 +741,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -979,15 +979,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="2:16">
       <c r="B2" s="1" t="s">
@@ -1059,10 +1059,10 @@
       <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="J8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="49"/>
+      <c r="K8" s="50"/>
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
       <c r="N8" s="10"/>
@@ -1767,7 +1767,7 @@
       <c r="B35" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="50" t="s">
+      <c r="C35" s="46" t="s">
         <v>144</v>
       </c>
       <c r="D35" s="18" t="s">
@@ -1777,10 +1777,10 @@
         <v>147</v>
       </c>
       <c r="F35" s="4">
-        <v>44391</v>
+        <v>44395</v>
       </c>
       <c r="G35" s="4">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="H35" s="27"/>
     </row>
@@ -1788,7 +1788,7 @@
       <c r="B36" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="46" t="s">
         <v>135</v>
       </c>
       <c r="D36" s="18" t="s">
@@ -1798,10 +1798,10 @@
         <v>25</v>
       </c>
       <c r="F36" s="4">
-        <v>44391</v>
+        <v>44395</v>
       </c>
       <c r="G36" s="4">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="H36" s="27"/>
     </row>
@@ -1819,10 +1819,10 @@
         <v>42</v>
       </c>
       <c r="F37" s="4">
-        <v>44391</v>
+        <v>44395</v>
       </c>
       <c r="G37" s="4">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="H37" s="27"/>
     </row>
@@ -1830,7 +1830,7 @@
       <c r="B38" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="46" t="s">
         <v>141</v>
       </c>
       <c r="D38" s="18" t="s">
@@ -1840,10 +1840,10 @@
         <v>127</v>
       </c>
       <c r="F38" s="4">
-        <v>44391</v>
+        <v>44395</v>
       </c>
       <c r="G38" s="4">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="H38" s="27"/>
     </row>
@@ -1851,7 +1851,7 @@
       <c r="B39" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="C39" s="50" t="s">
+      <c r="C39" s="46" t="s">
         <v>139</v>
       </c>
       <c r="D39" s="18" t="s">
@@ -1861,10 +1861,10 @@
         <v>48</v>
       </c>
       <c r="F39" s="4">
-        <v>44391</v>
+        <v>44395</v>
       </c>
       <c r="G39" s="4">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="H39" s="27"/>
     </row>
@@ -1882,10 +1882,10 @@
         <v>78</v>
       </c>
       <c r="F40" s="21">
-        <v>44397</v>
+        <v>44400</v>
       </c>
       <c r="G40" s="21">
-        <v>44398</v>
+        <v>44403</v>
       </c>
       <c r="H40" s="27"/>
     </row>
@@ -1903,10 +1903,10 @@
         <v>79</v>
       </c>
       <c r="F41" s="21">
-        <v>44398</v>
+        <v>44403</v>
       </c>
       <c r="G41" s="21">
-        <v>44400</v>
+        <v>44405</v>
       </c>
       <c r="H41" s="27"/>
     </row>
@@ -1924,10 +1924,10 @@
         <v>64</v>
       </c>
       <c r="F42" s="21">
-        <v>44400</v>
+        <v>44403</v>
       </c>
       <c r="G42" s="21">
-        <v>44403</v>
+        <v>44405</v>
       </c>
       <c r="H42" s="27"/>
     </row>

</xml_diff>

<commit_message>
Actualizando la Linea Base 3
</commit_message>
<xml_diff>
--- a/Documentos/SF/Cronograma/ST-CP.xlsx
+++ b/Documentos/SF/Cronograma/ST-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jota\Documents\DESARROLLO JOLLJA\FiveSolutions\Documentos\SF\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jota\Documents\DESARROLLO JOLLJA\Grupo5\FiveSolutions\Documentos\SF\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17CBDC3-A504-4F7F-AE49-53F8D11F642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CADBE7-32F1-4537-BBD0-97CA4B90E878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="153">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Zavaleta/DO,Centti/ARS</t>
   </si>
   <si>
-    <t>Sprint Review</t>
-  </si>
-  <si>
     <t>Sprint retrospective</t>
   </si>
   <si>
@@ -294,9 +291,6 @@
     <t>HU-Módulo de Interfáz principal</t>
   </si>
   <si>
-    <t>Módulo de Interfaz Principal</t>
-  </si>
-  <si>
     <t>ST-MIP</t>
   </si>
   <si>
@@ -475,6 +469,21 @@
   </si>
   <si>
     <t>HU-Validar productos y/o servicios (Administrador General)</t>
+  </si>
+  <si>
+    <t>ST-MIG</t>
+  </si>
+  <si>
+    <t>Módulo de Interfaz General</t>
+  </si>
+  <si>
+    <t>ST-SRT.DOCX</t>
+  </si>
+  <si>
+    <t>ST-SRS.DOC</t>
+  </si>
+  <si>
+    <t>ST-SRP.DOCX</t>
   </si>
 </sst>
 </file>
@@ -956,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P1009"/>
+  <dimension ref="B1:P1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1137,7 +1146,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>25</v>
@@ -1227,16 +1236,16 @@
     </row>
     <row r="14" spans="2:16" s="42" customFormat="1">
       <c r="B14" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="44" t="s">
         <v>113</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>115</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1328,7 +1337,7 @@
         <v>53</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F17" s="21">
         <v>44359</v>
@@ -1353,16 +1362,16 @@
     </row>
     <row r="18" spans="2:16">
       <c r="B18" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F18" s="21">
         <v>44363</v>
@@ -1387,13 +1396,13 @@
     </row>
     <row r="19" spans="2:16" s="43" customFormat="1">
       <c r="B19" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>25</v>
@@ -1417,16 +1426,16 @@
     </row>
     <row r="20" spans="2:16" s="43" customFormat="1">
       <c r="B20" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F20" s="21">
         <v>44363</v>
@@ -1447,13 +1456,13 @@
     </row>
     <row r="21" spans="2:16" s="43" customFormat="1">
       <c r="B21" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>25</v>
@@ -1477,16 +1486,16 @@
     </row>
     <row r="22" spans="2:16" s="35" customFormat="1">
       <c r="B22" s="19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C22" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="E22" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F22" s="21">
         <v>44363</v>
@@ -1505,16 +1514,16 @@
     </row>
     <row r="23" spans="2:16" s="35" customFormat="1">
       <c r="B23" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C23" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>134</v>
-      </c>
       <c r="E23" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F23" s="21">
         <v>44363</v>
@@ -1542,7 +1551,7 @@
         <v>60</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F24" s="21">
         <v>44367</v>
@@ -1665,7 +1674,7 @@
         <v>60</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>25</v>
@@ -1679,102 +1688,102 @@
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:16">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="16" t="s">
+      <c r="C30" s="12"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="B31" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="2:16" ht="15.75" customHeight="1">
+      <c r="B32" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="21">
-        <v>44376</v>
-      </c>
-      <c r="G30" s="21">
-        <v>44377</v>
-      </c>
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="2:16">
-      <c r="B31" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="2:16">
-      <c r="B32" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="13"/>
+      <c r="F32" s="4">
+        <v>44385</v>
+      </c>
+      <c r="G32" s="4">
+        <v>44386</v>
+      </c>
+      <c r="H32" s="27"/>
     </row>
     <row r="33" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B33" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>73</v>
+      <c r="B33" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>75</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>25</v>
+        <v>76</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="F33" s="4">
-        <v>44385</v>
+        <v>44387</v>
       </c>
       <c r="G33" s="4">
-        <v>44386</v>
+        <v>44389</v>
       </c>
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B34" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>76</v>
+    <row r="34" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B34" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="46" t="s">
+        <v>142</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>110</v>
+        <v>135</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="F34" s="4">
-        <v>44387</v>
+        <v>44395</v>
       </c>
       <c r="G34" s="4">
-        <v>44389</v>
+        <v>44400</v>
       </c>
       <c r="H34" s="27"/>
     </row>
     <row r="35" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="B35" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" s="46" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>147</v>
+        <v>134</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="F35" s="4">
         <v>44395</v>
@@ -1786,16 +1795,16 @@
     </row>
     <row r="36" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="B36" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="C36" s="46" t="s">
-        <v>135</v>
+        <v>105</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>106</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F36" s="4">
         <v>44395</v>
@@ -1805,18 +1814,18 @@
       </c>
       <c r="H36" s="27"/>
     </row>
-    <row r="37" spans="2:8" s="35" customFormat="1" ht="15.75" customHeight="1">
+    <row r="37" spans="2:8" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="B37" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>108</v>
+        <v>138</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>139</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="F37" s="4">
         <v>44395</v>
@@ -1828,16 +1837,16 @@
     </row>
     <row r="38" spans="2:8" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="B38" s="38" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C38" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D38" s="18" t="s">
-        <v>142</v>
-      </c>
       <c r="E38" s="19" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="F38" s="4">
         <v>44395</v>
@@ -1847,30 +1856,30 @@
       </c>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="2:8" s="45" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B39" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="46" t="s">
-        <v>139</v>
+    <row r="39" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B39" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" s="4">
-        <v>44395</v>
-      </c>
-      <c r="G39" s="4">
+        <v>60</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="21">
         <v>44400</v>
+      </c>
+      <c r="G39" s="21">
+        <v>44403</v>
       </c>
       <c r="H39" s="27"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" customHeight="1">
       <c r="B40" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>60</v>
@@ -1878,20 +1887,20 @@
       <c r="D40" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="41" t="s">
         <v>78</v>
       </c>
       <c r="F40" s="21">
-        <v>44400</v>
+        <v>44403</v>
       </c>
       <c r="G40" s="21">
-        <v>44403</v>
+        <v>44405</v>
       </c>
       <c r="H40" s="27"/>
     </row>
     <row r="41" spans="2:8" ht="15.75" customHeight="1">
       <c r="B41" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>60</v>
@@ -1899,8 +1908,8 @@
       <c r="D41" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="41" t="s">
-        <v>79</v>
+      <c r="E41" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="F41" s="21">
         <v>44403</v>
@@ -1912,7 +1921,7 @@
     </row>
     <row r="42" spans="2:8" ht="15.75" customHeight="1">
       <c r="B42" s="19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>60</v>
@@ -1927,13 +1936,13 @@
         <v>44403</v>
       </c>
       <c r="G42" s="21">
-        <v>44405</v>
+        <v>44404</v>
       </c>
       <c r="H42" s="27"/>
     </row>
     <row r="43" spans="2:8" ht="15.75" customHeight="1">
       <c r="B43" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>60</v>
@@ -1941,174 +1950,174 @@
       <c r="D43" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="22" t="s">
-        <v>64</v>
+      <c r="E43" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="F43" s="21">
-        <v>44403</v>
+        <v>44405</v>
       </c>
       <c r="G43" s="21">
-        <v>44404</v>
+        <v>44405</v>
       </c>
       <c r="H43" s="27"/>
     </row>
     <row r="44" spans="2:8" ht="15.75" customHeight="1">
       <c r="B44" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>67</v>
+        <v>151</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="F44" s="21">
-        <v>44405</v>
+        <v>44406</v>
       </c>
       <c r="G44" s="21">
-        <v>44405</v>
+        <v>44406</v>
       </c>
       <c r="H44" s="27"/>
     </row>
     <row r="45" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B45" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="16" t="s">
+      <c r="B45" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B46" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B47" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="21">
-        <v>44406</v>
-      </c>
-      <c r="G45" s="21">
-        <v>44406</v>
-      </c>
-      <c r="H45" s="27"/>
-    </row>
-    <row r="46" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B46" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="21">
-        <v>44405</v>
-      </c>
-      <c r="G46" s="21">
-        <v>44405</v>
-      </c>
-      <c r="H46" s="27"/>
-    </row>
-    <row r="47" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B47" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="12"/>
+      <c r="F47" s="4">
+        <v>44410</v>
+      </c>
+      <c r="G47" s="4">
+        <v>44411</v>
+      </c>
+      <c r="H47" s="27"/>
     </row>
     <row r="48" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B48" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="13"/>
+      <c r="B48" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F48" s="4">
+        <v>44411</v>
+      </c>
+      <c r="G48" s="4">
+        <v>44414</v>
+      </c>
+      <c r="H48" s="27"/>
     </row>
     <row r="49" spans="2:8" ht="15.75" customHeight="1">
       <c r="B49" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F49" s="4">
-        <v>44410</v>
-      </c>
-      <c r="G49" s="4">
-        <v>44411</v>
+        <v>87</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F49" s="21">
+        <v>44417</v>
+      </c>
+      <c r="G49" s="21">
+        <v>44419</v>
       </c>
       <c r="H49" s="27"/>
     </row>
     <row r="50" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B50" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="F50" s="4">
-        <v>44411</v>
-      </c>
-      <c r="G50" s="4">
-        <v>44414</v>
+      <c r="B50" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F50" s="21">
+        <v>44424</v>
+      </c>
+      <c r="G50" s="21">
+        <v>44426</v>
       </c>
       <c r="H50" s="27"/>
     </row>
     <row r="51" spans="2:8" ht="15.75" customHeight="1">
       <c r="B51" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>91</v>
+      <c r="E51" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="F51" s="21">
-        <v>44417</v>
+        <v>44424</v>
       </c>
       <c r="G51" s="21">
-        <v>44419</v>
+        <v>44426</v>
       </c>
       <c r="H51" s="27"/>
     </row>
     <row r="52" spans="2:8" ht="15.75" customHeight="1">
       <c r="B52" s="16" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>56</v>
@@ -2123,70 +2132,70 @@
     </row>
     <row r="53" spans="2:8" ht="15.75" customHeight="1">
       <c r="B53" s="16" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>56</v>
+        <v>99</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>101</v>
       </c>
       <c r="F53" s="21">
-        <v>44424</v>
+        <v>44426</v>
       </c>
       <c r="G53" s="21">
-        <v>44426</v>
+        <v>44428</v>
       </c>
       <c r="H53" s="27"/>
     </row>
     <row r="54" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B54" s="16" t="s">
-        <v>97</v>
+      <c r="B54" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>99</v>
+        <v>60</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>60</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="F54" s="21">
-        <v>44424</v>
+        <v>44428</v>
       </c>
       <c r="G54" s="21">
-        <v>44426</v>
+        <v>44429</v>
       </c>
       <c r="H54" s="27"/>
     </row>
     <row r="55" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B55" s="16" t="s">
-        <v>100</v>
+      <c r="B55" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E55" s="40" t="s">
-        <v>103</v>
+        <v>60</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="F55" s="21">
-        <v>44426</v>
+        <v>44429</v>
       </c>
       <c r="G55" s="21">
-        <v>44428</v>
+        <v>44431</v>
       </c>
       <c r="H55" s="27"/>
     </row>
     <row r="56" spans="2:8" ht="15.75" customHeight="1">
       <c r="B56" s="19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>60</v>
@@ -2195,19 +2204,19 @@
         <v>60</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="F56" s="21">
-        <v>44428</v>
+        <v>44431</v>
       </c>
       <c r="G56" s="21">
-        <v>44429</v>
+        <v>44434</v>
       </c>
       <c r="H56" s="27"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" customHeight="1">
       <c r="B57" s="19" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>60</v>
@@ -2215,20 +2224,20 @@
       <c r="D57" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="16" t="s">
-        <v>79</v>
+      <c r="E57" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="F57" s="21">
-        <v>44429</v>
+        <v>44434</v>
       </c>
       <c r="G57" s="21">
-        <v>44431</v>
+        <v>44435</v>
       </c>
       <c r="H57" s="27"/>
     </row>
     <row r="58" spans="2:8" ht="15.75" customHeight="1">
       <c r="B58" s="19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>60</v>
@@ -2236,121 +2245,61 @@
       <c r="D58" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="16" t="s">
-        <v>64</v>
+      <c r="E58" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="F58" s="21">
-        <v>44431</v>
+        <v>44436</v>
       </c>
       <c r="G58" s="21">
-        <v>44434</v>
+        <v>44436</v>
       </c>
       <c r="H58" s="27"/>
     </row>
     <row r="59" spans="2:8" ht="15.75" customHeight="1">
       <c r="B59" s="19" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>64</v>
+        <v>150</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="F59" s="21">
-        <v>44434</v>
+        <v>44437</v>
       </c>
       <c r="G59" s="21">
-        <v>44435</v>
+        <v>44437</v>
       </c>
       <c r="H59" s="27"/>
     </row>
     <row r="60" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B60" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F60" s="21">
-        <v>44436</v>
-      </c>
-      <c r="G60" s="21">
-        <v>44436</v>
-      </c>
-      <c r="H60" s="27"/>
+      <c r="B60" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="12"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="12"/>
     </row>
     <row r="61" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B61" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F61" s="21">
-        <v>44437</v>
-      </c>
-      <c r="G61" s="21">
-        <v>44437</v>
-      </c>
-      <c r="H61" s="27"/>
-    </row>
-    <row r="62" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B62" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F62" s="21">
-        <v>44436</v>
-      </c>
-      <c r="G62" s="21">
-        <v>44436</v>
-      </c>
-      <c r="H62" s="27"/>
-    </row>
-    <row r="63" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B63" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="12"/>
-    </row>
-    <row r="64" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B64" s="12"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="15"/>
-    </row>
+      <c r="B61" s="12"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="15"/>
+    </row>
+    <row r="62" spans="2:8" ht="15.75" customHeight="1"/>
+    <row r="63" spans="2:8" ht="15.75" customHeight="1"/>
+    <row r="64" spans="2:8" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -3293,9 +3242,6 @@
     <row r="1004" ht="15.75" customHeight="1"/>
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
-    <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:H1"/>

</xml_diff>